<commit_message>
Layout Cronograma - Excel
</commit_message>
<xml_diff>
--- a/EDT y Cronograma/Cronograma.xlsx
+++ b/EDT y Cronograma/Cronograma.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodas/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08640A33-EAE7-EA46-8306-4F3D9958C897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Folha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +25,78 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+  <si>
+    <t>Semana 1</t>
+  </si>
+  <si>
+    <t>Semana 2</t>
+  </si>
+  <si>
+    <t>Semana 3</t>
+  </si>
+  <si>
+    <t>Semana 4</t>
+  </si>
+  <si>
+    <t>Semana 5</t>
+  </si>
+  <si>
+    <t>Semana 6</t>
+  </si>
+  <si>
+    <t>Semana 7</t>
+  </si>
+  <si>
+    <t>Semana 8</t>
+  </si>
+  <si>
+    <t>Semana 9</t>
+  </si>
+  <si>
+    <t>Semana 10</t>
+  </si>
+  <si>
+    <t>Semana 11</t>
+  </si>
+  <si>
+    <t>Semana 12</t>
+  </si>
+  <si>
+    <t>Semana 13</t>
+  </si>
+  <si>
+    <t>Francisco Rodrigues</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis </t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>Equipo 1</t>
+  </si>
+  <si>
+    <t>Equipo 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparacion de Propuestas
+</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +104,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (corpo)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -45,12 +153,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +543,351 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="63">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A7B446F-75EB-1042-AE7D-9A46F0B33CCA}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="61" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="8" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" ht="61" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>